<commit_message>
[IMP] Add supplier receipt follow up report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
@@ -221,7 +221,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -229,7 +229,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -253,7 +253,7 @@
   <dimension ref="A1:V1124"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[IMP] Adjust Advance Payment Report
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Account Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Report Date</t>
+    <t xml:space="preserve">As of Date</t>
   </si>
   <si>
     <t xml:space="preserve">Run By</t>
@@ -110,8 +110,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\)"/>
-    <numFmt numFmtId="167" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="#,###.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0"/>
   </numFmts>
   <fonts count="5">
     <font>

</xml_diff>

<commit_message>
#3438 - insert field on excel
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\jasper\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Advance Payment Report</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Account Name</t>
+  </si>
+  <si>
+    <t>Journal Number</t>
   </si>
 </sst>
 </file>
@@ -584,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMM8"/>
+  <dimension ref="A1:AMN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -602,57 +605,57 @@
     <col min="8" max="8" width="27.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="23.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="33.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="39.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="31.42578125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="31.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="28" style="2" customWidth="1"/>
-    <col min="16" max="16" width="20.140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="4" customWidth="1"/>
-    <col min="18" max="18" width="17.140625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="23.42578125" style="3" customWidth="1"/>
-    <col min="20" max="20" width="24.85546875" style="3" customWidth="1"/>
-    <col min="21" max="21" width="26.140625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="26" style="3" customWidth="1"/>
-    <col min="23" max="23" width="26.28515625" style="3" customWidth="1"/>
-    <col min="24" max="24" width="27.7109375" style="3" customWidth="1"/>
-    <col min="25" max="1027" width="11.5703125" style="5"/>
+    <col min="11" max="12" width="33.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="39.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="31.42578125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="28" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="17.140625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="24.85546875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="26.140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="26" style="3" customWidth="1"/>
+    <col min="24" max="24" width="26.28515625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="27.7109375" style="3" customWidth="1"/>
+    <col min="26" max="1028" width="11.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6"/>
     </row>
-    <row r="2" spans="1:24" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
@@ -687,42 +690,45 @@
         <v>13</v>
       </c>
       <c r="L8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="N8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="Q8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="R8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="S8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="T8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="U8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="U8" s="12" t="s">
+      <c r="V8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="12" t="s">
+      <c r="W8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="W8" s="12" t="s">
+      <c r="X8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="X8" s="12" t="s">
+      <c r="Y8" s="12" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#3438 - update xlsx file
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
@@ -16,6 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_SECOND_FORMAT" hidden="1">" "</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -589,20 +590,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="27.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="33.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="23.140625" style="2" customWidth="1"/>
     <col min="11" max="12" width="33.5703125" style="2" customWidth="1"/>
@@ -623,62 +623,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="F8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H8" s="11" t="s">
         <v>9</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>10</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
#3697_Advance_Payment module : pabi_account_report FI : รายงาน Advance Payment ย้ายคอลัมน์ และเพิ่มคอลัมน์ ISSUES : https://mobileapp.nstda.or.th/redmine/issues/3697
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_advance_payment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\801645\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_SECOND_FORMAT" hidden="1">" "</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Advance Payment Report</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Journal Number</t>
+  </si>
+  <si>
+    <t>Document Date</t>
+  </si>
+  <si>
+    <t>Posting Date</t>
   </si>
 </sst>
 </file>
@@ -590,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -610,8 +616,8 @@
     <col min="14" max="14" width="31.42578125" style="3" customWidth="1"/>
     <col min="15" max="15" width="31.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="28" style="2" customWidth="1"/>
-    <col min="17" max="17" width="20.140625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="28.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="26.7109375" style="4" customWidth="1"/>
     <col min="19" max="19" width="17.140625" style="3" customWidth="1"/>
     <col min="20" max="20" width="23.42578125" style="3" customWidth="1"/>
     <col min="21" max="21" width="24.85546875" style="3" customWidth="1"/>
@@ -619,48 +625,50 @@
     <col min="23" max="23" width="26" style="3" customWidth="1"/>
     <col min="24" max="24" width="26.28515625" style="3" customWidth="1"/>
     <col min="25" max="25" width="27.7109375" style="3" customWidth="1"/>
-    <col min="26" max="1028" width="11.5703125" style="5"/>
+    <col min="26" max="26" width="27.85546875" style="5" customWidth="1"/>
+    <col min="27" max="27" width="28.140625" style="5" customWidth="1"/>
+    <col min="28" max="1028" width="11.5703125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
     </row>
-    <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
     </row>
-    <row r="6" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="10"/>
     </row>
-    <row r="7" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
@@ -680,60 +688,66 @@
         <v>10</v>
       </c>
       <c r="G8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="O8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="N8" s="11" t="s">
+      <c r="P8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="R8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="S8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="R8" s="12" t="s">
+      <c r="T8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="U8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="V8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="U8" s="12" t="s">
+      <c r="W8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="V8" s="12" t="s">
+      <c r="X8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="W8" s="12" t="s">
+      <c r="Y8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="X8" s="12" t="s">
+      <c r="Z8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="Y8" s="12" t="s">
+      <c r="AA8" s="12" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>